<commit_message>
Dash atualizadada com uma nova linha de requisito
</commit_message>
<xml_diff>
--- a/Documentação/Documentação/TI-Backlog-Grupo10 V1.xlsx
+++ b/Documentação/Documentação/TI-Backlog-Grupo10 V1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lioci\Desktop\28.10 Projet\projeto-pi\Documentação\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4ED5B2-1622-4B29-B293-64ED7443D732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EB33641-A011-4B90-A368-B195E8257783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{0E4C50FC-4743-41E1-8EF2-E2C48055392E}"/>
   </bookViews>
@@ -19,9 +19,9 @@
     <sheet name="SPRINT3Backlog" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BackLog!$A$2:$J$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BackLog!$A$2:$J$45</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="134">
+  <si>
+    <t>SafeWare - Backlog</t>
+  </si>
   <si>
     <t>Requisito</t>
   </si>
@@ -65,374 +68,383 @@
     <t>SPRINT</t>
   </si>
   <si>
-    <t>SafeWare - Backlog</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>Responsavel</t>
   </si>
   <si>
+    <t>Área</t>
+  </si>
+  <si>
+    <t>Planejado</t>
+  </si>
+  <si>
+    <t>Realizado</t>
+  </si>
+  <si>
     <t>Criação do github</t>
   </si>
   <si>
     <t>Criação do github e upload de todos os arquivos.</t>
   </si>
   <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>SPRINT1</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>Tiago</t>
+  </si>
+  <si>
+    <t>Pesquisa e Inovação</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Documentação</t>
   </si>
   <si>
     <t>Contexto e justificativa do projeto.</t>
   </si>
   <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>Erik</t>
+  </si>
+  <si>
     <t>Diagrama</t>
   </si>
   <si>
     <t>Diagrama de visão de negócio.</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Bhreno</t>
+  </si>
+  <si>
+    <t>SPRINT2</t>
+  </si>
+  <si>
     <t>Protótipo do site</t>
   </si>
   <si>
     <t>Protótipo do site feito no figma.</t>
   </si>
   <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Viviane</t>
+  </si>
+  <si>
+    <t>SPRINT3</t>
+  </si>
+  <si>
     <t>Simulador financeiro</t>
   </si>
   <si>
     <t>Tela sem CSS do simulador financeiro.</t>
   </si>
   <si>
+    <t>Kaio</t>
+  </si>
+  <si>
+    <t>Algoritimos</t>
+  </si>
+  <si>
+    <t>SPRINT4</t>
+  </si>
+  <si>
+    <t>Trello configurado e populado</t>
+  </si>
+  <si>
     <t>Trello configurado e com todos os requisitos da sprint atual.</t>
   </si>
   <si>
-    <t>Trello configurado e populado</t>
+    <t>Tecnologia da informação</t>
+  </si>
+  <si>
+    <t>Média</t>
   </si>
   <si>
     <t>Documentação com o contexto, justificativa, objetivo e escopo do projeto.</t>
   </si>
   <si>
+    <t>Banco de dados</t>
+  </si>
+  <si>
     <t>Tabelas criadas no MySQL</t>
   </si>
   <si>
-    <t>Banco de dados</t>
+    <t>Banco de Dados</t>
   </si>
   <si>
     <t>Instalação e configuração do Arduíno</t>
   </si>
   <si>
+    <t>Instalação e configuração do arduíno feito no IDE Arduíno</t>
+  </si>
+  <si>
+    <t>Arquitetura Computacional</t>
+  </si>
+  <si>
     <t>Instalação da VM local</t>
   </si>
   <si>
     <t>Instalação e configuração da VM.</t>
   </si>
   <si>
-    <t>SPRINT1</t>
-  </si>
-  <si>
-    <t>SPRINT2</t>
-  </si>
-  <si>
-    <t>SPRINT3</t>
-  </si>
-  <si>
-    <t>Feito</t>
+    <t>Introdução a Sistemas Operacionais</t>
+  </si>
+  <si>
+    <t>Atualização do projeto no github</t>
+  </si>
+  <si>
+    <t>Atualizar todos os arquivos do projeto no GitHub.</t>
   </si>
   <si>
     <t>Em andamento</t>
   </si>
   <si>
-    <t>Tiago</t>
-  </si>
-  <si>
-    <t>Viviane</t>
-  </si>
-  <si>
-    <t>Erik</t>
-  </si>
-  <si>
-    <t>Bhreno</t>
-  </si>
-  <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
-    <t>Desejável</t>
-  </si>
-  <si>
-    <t>Atualização do projeto no github</t>
-  </si>
-  <si>
     <t>Planilha de riscos</t>
   </si>
   <si>
+    <t>Análise de riscos e consequencias.</t>
+  </si>
+  <si>
     <t>Especificação da dashboard</t>
   </si>
   <si>
+    <t>Especificar quais gráficos e KPIs que serão apresentadas na dashboard.</t>
+  </si>
+  <si>
     <t>Site estatico institucional</t>
   </si>
   <si>
+    <t>Site estático e local feito em HTML e CSS.</t>
+  </si>
+  <si>
     <t>Site estatico dashboard</t>
   </si>
   <si>
+    <t>Dashboard estática feito em HTML e CSS.</t>
+  </si>
+  <si>
+    <t>Página de login</t>
+  </si>
+  <si>
+    <t>Criação da pagina de login em HTML e CSS.</t>
+  </si>
+  <si>
+    <t>Página de cadastro</t>
+  </si>
+  <si>
+    <t>Criação da pagina de cadastro em HTML e CSS.</t>
+  </si>
+  <si>
     <t>Diagrama de solução</t>
   </si>
   <si>
+    <t>Arquitetura técnica do projeto.</t>
+  </si>
+  <si>
     <t>Organização da ferramenta de gestão</t>
   </si>
   <si>
+    <t>Sprints e atividades organizadas na ferramenta de gestão.</t>
+  </si>
+  <si>
+    <t>Integrantes</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
     <t>BackLog da SPRINT</t>
   </si>
   <si>
+    <t>Demanda, pontuação e prioridade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bhreno Venditti de Oliveira Barboza </t>
+  </si>
+  <si>
     <t>Modelagem lógica do projeto</t>
   </si>
   <si>
+    <t>Modelagem lógica do banco de dados.</t>
+  </si>
+  <si>
+    <t>Erik Cecílio</t>
+  </si>
+  <si>
     <t>Simular a integração do sistema</t>
   </si>
   <si>
+    <t>Simulação da integração do sistema usando o sensor e gráfico.</t>
+  </si>
+  <si>
+    <t>Kaio Kenuy da Silva Hergesel</t>
+  </si>
+  <si>
     <t>Usar API local</t>
   </si>
   <si>
+    <t>Usar a API para a integração do sensor.</t>
+  </si>
+  <si>
+    <t>Tiago Bezerril Moreira</t>
+  </si>
+  <si>
     <t>Instalar MySQL na VMLinux local</t>
   </si>
   <si>
+    <t>Instalação do MySQL na VMLinux na mesma máquina.</t>
+  </si>
+  <si>
+    <t>Viviane dos Santos</t>
+  </si>
+  <si>
     <t>Validar a solução técnica</t>
   </si>
   <si>
-    <t>Página de cadastro</t>
-  </si>
-  <si>
-    <t>Página de login</t>
-  </si>
-  <si>
-    <t>Criação da pagina de cadastro em HTML e CSS.</t>
-  </si>
-  <si>
-    <t>Criação da pagina de login em HTML e CSS.</t>
-  </si>
-  <si>
-    <t>Dashboard estática feito em HTML e CSS.</t>
-  </si>
-  <si>
-    <t>Site estático e local feito em HTML e CSS.</t>
-  </si>
-  <si>
-    <t>Análise de riscos e consequencias.</t>
-  </si>
-  <si>
-    <t>Atualizar todos os arquivos do projeto no GitHub.</t>
-  </si>
-  <si>
-    <t>Arquitetura técnica do projeto.</t>
-  </si>
-  <si>
-    <t>Demanda, pontuação e prioridade.</t>
-  </si>
-  <si>
-    <t>Sprints e atividades organizadas na ferramenta de gestão.</t>
-  </si>
-  <si>
-    <t>Usar a API para a integração do sensor.</t>
-  </si>
-  <si>
-    <t>Instalação do MySQL na VMLinux na mesma máquina.</t>
-  </si>
-  <si>
     <t>Validar a solução técnica com o cliente.</t>
   </si>
   <si>
-    <t>Área</t>
-  </si>
-  <si>
-    <t>Pesquisa e Inovação</t>
-  </si>
-  <si>
-    <t>Algoritimos</t>
-  </si>
-  <si>
-    <t>Tecnologia da informação</t>
-  </si>
-  <si>
-    <t>Arquitetura Computacional</t>
-  </si>
-  <si>
-    <t>Banco de Dados</t>
-  </si>
-  <si>
-    <t>Introdução a Sistemas Operacionais</t>
-  </si>
-  <si>
     <t>Fluxograma de suporte</t>
   </si>
   <si>
+    <t>Fluxograma de suporte.</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
     <t>Ferramente de Help Desk</t>
   </si>
   <si>
+    <t>Ferramente de Help Desk.</t>
+  </si>
+  <si>
     <t>Documento de mudança</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>GG</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>Pendente</t>
-  </si>
-  <si>
-    <t>Kaio</t>
-  </si>
-  <si>
-    <t>Realizado</t>
-  </si>
-  <si>
-    <t>Planejado</t>
-  </si>
-  <si>
-    <t>SPRINT4</t>
+    <t>Documento de mudança.</t>
   </si>
   <si>
     <t>Infraestrutura simulada de cliente na VM</t>
+  </si>
+  <si>
+    <t>Infraestrutura simulada de cliente na maquina virtual.</t>
+  </si>
+  <si>
+    <t>Aplicação funcionando</t>
+  </si>
+  <si>
+    <t>Ter uma maquina só com o banco outra com os dados coletados pelo sensor e o cliente acessando nosso site da maquina dele.</t>
   </si>
   <si>
     <t>Modelagem Lógica e
 Script SQL Server</t>
   </si>
   <si>
+    <t>Modelagem Lógica e Script MySQL Server.</t>
+  </si>
+  <si>
     <t>Teste integrado do analytics</t>
   </si>
   <si>
+    <t>Teste integrado do analytics.</t>
+  </si>
+  <si>
     <t>Teste integrado da solução de IoT</t>
   </si>
   <si>
+    <t>Teste integrado da solução de IoT.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Teste integrado (Arduíno + DB)</t>
   </si>
   <si>
+    <t xml:space="preserve"> Teste integrado do arduíno e do banco de dados.</t>
+  </si>
+  <si>
     <t>Data Acqu Ino + BobIA (N3)</t>
   </si>
   <si>
-    <t>Instalação e configuração do arduíno feito no IDE Arduíno</t>
-  </si>
-  <si>
-    <t>Especificar quais gráficos e KPIs que serão apresentadas na dashboard.</t>
-  </si>
-  <si>
-    <t>Modelagem lógica do banco de dados.</t>
-  </si>
-  <si>
-    <t>Simulação da integração do sistema usando o sensor e gráfico.</t>
+    <t>Data Acqu Ino + BobIA (N3).</t>
   </si>
   <si>
     <t>Tabelas criadas no banco de dados (Final)</t>
   </si>
   <si>
+    <t>Versão final das tabelas criadas no banco de dados.</t>
+  </si>
+  <si>
     <t>Manual de instalação</t>
   </si>
   <si>
+    <t>Manual para instalação dos sensores e todo o sistema.</t>
+  </si>
+  <si>
     <t>Documentação do projeto atualizada</t>
   </si>
   <si>
+    <t>Documentação do projeto atualizada.</t>
+  </si>
+  <si>
     <t>PPT de apresentação do projeto</t>
   </si>
   <si>
+    <t>PPT de apresentação do projeto.</t>
+  </si>
+  <si>
     <t>Dashboard(ChartJS) acessando o banco</t>
   </si>
   <si>
+    <t>Dashboard feita com ChartJS acessando o banco.</t>
+  </si>
+  <si>
+    <t>Site institucional</t>
+  </si>
+  <si>
+    <t>Versão final do site institucional.</t>
+  </si>
+  <si>
+    <t>Cadastro e login acessando o banco</t>
+  </si>
+  <si>
+    <t>Cadastro e login acessando o banco.(Web-Dat-viz)</t>
+  </si>
+  <si>
     <t>Individual - Indicadores acessando o banco</t>
   </si>
   <si>
-    <t>Cadastro e login acessando o banco</t>
-  </si>
-  <si>
-    <t>Site institucional</t>
-  </si>
-  <si>
-    <t>Infraestrutura simulada de cliente na maquina virtual.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Teste integrado do arduíno e do banco de dados.</t>
-  </si>
-  <si>
-    <t>Versão final das tabelas criadas no banco de dados.</t>
-  </si>
-  <si>
-    <t>Manual para instalação dos sensores e todo o sistema.</t>
-  </si>
-  <si>
-    <t>Documentação do projeto atualizada.</t>
-  </si>
-  <si>
-    <t>PPT de apresentação do projeto.</t>
-  </si>
-  <si>
-    <t>Dashboard feita com ChartJS acessando o banco.</t>
-  </si>
-  <si>
-    <t>Versão final do site institucional.</t>
+    <t>Individual - Indicadores acessando o banco.</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>Modelagem Lógica e Script SQL Server.</t>
   </si>
   <si>
     <t>Cadastro e login acessando o banco.</t>
-  </si>
-  <si>
-    <t>Individual - Indicadores acessando o banco.</t>
-  </si>
-  <si>
-    <t>Fluxograma de suporte.</t>
-  </si>
-  <si>
-    <t>Ferramente de Help Desk.</t>
-  </si>
-  <si>
-    <t>Documento de mudança.</t>
-  </si>
-  <si>
-    <t>Modelagem Lógica e Script SQL Server.</t>
-  </si>
-  <si>
-    <t>Teste integrado do analytics.</t>
-  </si>
-  <si>
-    <t>Teste integrado da solução de IoT.</t>
-  </si>
-  <si>
-    <t>Data Acqu Ino + BobIA (N3).</t>
-  </si>
-  <si>
-    <t>Integrantes</t>
-  </si>
-  <si>
-    <t>Erik Cecílio</t>
-  </si>
-  <si>
-    <t>Viviane dos Santos</t>
-  </si>
-  <si>
-    <t>RA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bhreno Venditti de Oliveira Barboza </t>
-  </si>
-  <si>
-    <t>Tiago Bezerril Moreira</t>
-  </si>
-  <si>
-    <t>Kaio Kenuy da Silva Hergesel</t>
   </si>
 </sst>
 </file>
@@ -1663,7 +1675,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1713,7 +1725,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1747,11 +1759,48 @@
           <c:cat>
             <c:strRef>
               <c:f>BackLog!$L$3:$L$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SPRINT1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SPRINT2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SPRINT3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SPRINT4</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>BackLog!$M$3:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>158.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>158.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>158.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1801,7 +1850,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1835,11 +1884,48 @@
           <c:cat>
             <c:strRef>
               <c:f>BackLog!$L$3:$L$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SPRINT1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SPRINT2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SPRINT3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SPRINT4</c:v>
+                </c:pt>
+              </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>BackLog!$N$3:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
@@ -1857,7 +1943,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1814549743"/>
         <c:axId val="1814548303"/>
@@ -1903,7 +1988,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1814548303"/>
@@ -1949,7 +2034,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1814549743"/>
@@ -2001,7 +2086,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2039,7 +2124,7 @@
           <a:latin typeface="Inter"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2964,11 +3049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F959334-FF27-4A0F-9E6B-19A8615EAC13}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2991,7 +3075,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="27" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -3005,25 +3089,25 @@
     </row>
     <row r="2" spans="1:14" ht="21" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
@@ -3032,28 +3116,28 @@
         <v>9</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="L2" s="60"/>
       <c r="M2" s="32" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="32.1" customHeight="1">
       <c r="A3" s="24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8">
         <v>5</v>
@@ -3062,41 +3146,41 @@
         <v>3</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="L3" s="32" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="M3" s="59">
         <f>SUM(N4:N7)</f>
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="N3" s="59">
         <f>SUM(N4:N7)</f>
-        <v>462</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="32.1" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E4" s="9">
         <v>21</v>
@@ -3105,41 +3189,41 @@
         <v>1</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="M4" s="51">
         <f>N3/3</f>
-        <v>154</v>
+        <v>158.33333333333334</v>
       </c>
       <c r="N4" s="8">
-        <f>SUMIF($G$3:$G$35,L4,$E$3:$E$35)</f>
+        <f>SUMIF($G$3:$G$36,L4,$E$3:$E$36)</f>
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+    <row r="5" spans="1:14" ht="32.1" customHeight="1">
       <c r="A5" s="24" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E5" s="9">
         <v>8</v>
@@ -3148,41 +3232,41 @@
         <v>2</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M5" s="51">
         <f>N3/3</f>
-        <v>154</v>
+        <v>158.33333333333334</v>
       </c>
       <c r="N5" s="8">
-        <f>SUMIF($G$3:$G$35,L5,$E$3:$E$35)</f>
+        <f>SUMIF($G$3:$G$36,L5,$E$3:$E$36)</f>
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+    <row r="6" spans="1:14" ht="32.1" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8">
         <v>13</v>
@@ -3191,41 +3275,41 @@
         <v>2</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M6" s="51">
         <f>N3/3</f>
-        <v>154</v>
+        <v>158.33333333333334</v>
       </c>
       <c r="N6" s="8">
-        <f>SUMIF($G$3:$G$44,L6,$E$3:$E$44)</f>
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+        <f>SUMIF($G$3:$G$45,L6,$E$3:$E$45)</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="32.1" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E7" s="13">
         <v>21</v>
@@ -3234,19 +3318,19 @@
         <v>1</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="M7" s="8">
         <v>0</v>
@@ -3255,18 +3339,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+    <row r="8" spans="1:14" ht="32.1" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>8</v>
@@ -3275,41 +3359,41 @@
         <v>3</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="L8" s="32" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="M8" s="50">
         <f>AVERAGE(N4:N6)</f>
-        <v>154</v>
+        <v>158.33333333333334</v>
       </c>
       <c r="N8" s="50">
         <f>AVERAGE(N4:N6)</f>
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+        <v>158.33333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="32.1" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5">
         <v>21</v>
@@ -3318,30 +3402,30 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="32.1" customHeight="1">
       <c r="A10" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="42" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>80</v>
       </c>
       <c r="E10" s="4">
         <v>21</v>
@@ -3350,30 +3434,30 @@
         <v>2</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="32.1" customHeight="1">
+      <c r="A11" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="40" t="s">
         <v>28</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="32.1" hidden="1" customHeight="1">
-      <c r="A11" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>81</v>
       </c>
       <c r="E11" s="5">
         <v>8</v>
@@ -3382,30 +3466,30 @@
         <v>2</v>
       </c>
       <c r="G11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="32.1" customHeight="1">
+      <c r="A12" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="40" t="s">
         <v>28</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="32.1" hidden="1" customHeight="1">
-      <c r="A12" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>81</v>
       </c>
       <c r="E12" s="17">
         <v>8</v>
@@ -3414,31 +3498,31 @@
         <v>3</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H12" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="L12" s="58"/>
     </row>
     <row r="13" spans="1:14" ht="32.1" customHeight="1">
       <c r="A13" s="26" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E13" s="17">
         <v>8</v>
@@ -3447,31 +3531,31 @@
         <v>1</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H13" s="44" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="L13" s="58"/>
     </row>
-    <row r="14" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+    <row r="14" spans="1:14" ht="32.1" customHeight="1">
       <c r="A14" s="24" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E14" s="17">
         <v>8</v>
@@ -3480,31 +3564,31 @@
         <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H14" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I14" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="58"/>
+    </row>
+    <row r="15" spans="1:14" ht="32.1" customHeight="1">
+      <c r="A15" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="41" t="s">
         <v>33</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L14" s="58"/>
-    </row>
-    <row r="15" spans="1:14" ht="32.1" hidden="1" customHeight="1">
-      <c r="A15" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>82</v>
       </c>
       <c r="E15" s="8">
         <v>13</v>
@@ -3513,31 +3597,31 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="J15" s="12" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="L15" s="58"/>
     </row>
-    <row r="16" spans="1:14" ht="32.1" hidden="1" customHeight="1">
+    <row r="16" spans="1:14" ht="32.1" customHeight="1">
       <c r="A16" s="27" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E16" s="8">
         <v>13</v>
@@ -3546,30 +3630,30 @@
         <v>2</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="J16" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="32.1" customHeight="1">
       <c r="A17" s="24" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E17" s="8">
         <v>13</v>
@@ -3578,30 +3662,30 @@
         <v>1</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="32.1" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E18" s="8">
         <v>13</v>
@@ -3610,30 +3694,30 @@
         <v>2</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="32.1" customHeight="1">
+      <c r="A19" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="32.1" hidden="1" customHeight="1">
-      <c r="A19" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="C19" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E19" s="8">
         <v>13</v>
@@ -3642,30 +3726,30 @@
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="2" customFormat="1" ht="32.1" hidden="1" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="2" customFormat="1" ht="32.1" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E20" s="17">
         <v>8</v>
@@ -3674,32 +3758,32 @@
         <v>1</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H20" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+    <row r="21" spans="1:15" ht="32.1" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4">
         <v>8</v>
@@ -3708,38 +3792,38 @@
         <v>2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H21" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="L21" s="67" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="M21" s="68"/>
       <c r="N21" s="61" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="O21" s="62"/>
     </row>
-    <row r="22" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+    <row r="22" spans="1:15" ht="32.1" customHeight="1">
       <c r="A22" s="26" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E22" s="8">
         <v>13</v>
@@ -3748,37 +3832,37 @@
         <v>1</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H22" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="L22" s="63" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="M22" s="63"/>
       <c r="N22" s="31">
         <v>1242072</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+    <row r="23" spans="1:15" ht="32.1" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E23" s="17">
         <v>8</v>
@@ -3787,37 +3871,37 @@
         <v>3</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H23" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="L23" s="63" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="M23" s="63"/>
       <c r="N23" s="31">
         <v>1242121</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+    <row r="24" spans="1:15" ht="32.1" customHeight="1">
       <c r="A24" s="26" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E24" s="8">
         <v>13</v>
@@ -3826,37 +3910,37 @@
         <v>1</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H24" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L24" s="63" t="s">
         <v>84</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="L24" s="63" t="s">
-        <v>129</v>
       </c>
       <c r="M24" s="63"/>
       <c r="N24" s="31">
         <v>1242060</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+    <row r="25" spans="1:15" ht="32.1" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E25" s="8">
         <v>13</v>
@@ -3865,37 +3949,37 @@
         <v>2</v>
       </c>
       <c r="G25" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="J25" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="L25" s="63" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="M25" s="63"/>
       <c r="N25" s="31">
         <v>1242007</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="32.1" hidden="1" customHeight="1">
+    <row r="26" spans="1:15" ht="32.1" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E26" s="17">
         <v>8</v>
@@ -3904,37 +3988,37 @@
         <v>3</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H26" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I26" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="L26" s="63" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="M26" s="63"/>
       <c r="N26" s="31">
         <v>1242050</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="31.5" hidden="1" customHeight="1">
+    <row r="27" spans="1:15" ht="31.5" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E27" s="8">
         <v>13</v>
@@ -3943,30 +4027,30 @@
         <v>1</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H27" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="35.1" hidden="1" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="35.1" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="B28" s="52" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E28" s="4">
         <v>8</v>
@@ -3975,30 +4059,30 @@
         <v>1</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H28" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I28" s="31" t="s">
         <v>34</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="35.1" hidden="1" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="35.1" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B29" s="54" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E29" s="4">
         <v>8</v>
@@ -4007,30 +4091,30 @@
         <v>1</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H29" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="35.1" hidden="1" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="35.1" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="B30" s="54" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E30" s="8">
         <v>13</v>
@@ -4039,30 +4123,30 @@
         <v>1</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H30" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I30" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="35.1" hidden="1" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="35.1" customHeight="1">
       <c r="A31" s="53" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B31" s="55" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E31" s="4">
         <v>8</v>
@@ -4071,62 +4155,62 @@
         <v>1</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H31" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I31" s="31" t="s">
         <v>34</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="35.1" hidden="1" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="57.75">
       <c r="A32" s="53" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="E32" s="4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F32" s="31">
         <v>1</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H32" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="35.1" hidden="1" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="35.1" customHeight="1">
       <c r="A33" s="53" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B33" s="55" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E33" s="4">
         <v>8</v>
@@ -4135,30 +4219,30 @@
         <v>1</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H33" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="35.1" hidden="1" customHeight="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="35.1" customHeight="1">
       <c r="A34" s="53" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -4167,62 +4251,62 @@
         <v>1</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H34" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="35.1" hidden="1" customHeight="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="35.1" customHeight="1">
       <c r="A35" s="53" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B35" s="55" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="8">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="E35" s="4">
+        <v>8</v>
       </c>
       <c r="F35" s="31">
         <v>1</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H35" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I35" s="31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.5" hidden="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="35.1" customHeight="1">
       <c r="A36" s="53" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B36" s="55" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E36" s="8">
         <v>13</v>
@@ -4231,190 +4315,190 @@
         <v>1</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H36" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I36" s="31" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="28.5">
       <c r="A37" s="53" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B37" s="55" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="4">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="E37" s="8">
+        <v>13</v>
       </c>
       <c r="F37" s="31">
         <v>1</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H37" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="30" customHeight="1">
       <c r="A38" s="53" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B38" s="55" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="8">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="E38" s="4">
+        <v>8</v>
       </c>
       <c r="F38" s="31">
         <v>1</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H38" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I38" s="31" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30" customHeight="1">
       <c r="A39" s="53" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B39" s="55" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C39" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="4">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="E39" s="8">
+        <v>13</v>
       </c>
       <c r="F39" s="31">
         <v>1</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H39" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I39" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="30" customHeight="1">
       <c r="A40" s="53" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" s="8">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="E40" s="4">
+        <v>8</v>
       </c>
       <c r="F40" s="31">
         <v>1</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H40" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I40" s="31" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="30" customHeight="1">
       <c r="A41" s="53" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="E41" s="8">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F41" s="31">
         <v>1</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H41" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30" customHeight="1">
       <c r="A42" s="53" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B42" s="55" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E42" s="8">
         <v>13</v>
@@ -4423,62 +4507,62 @@
         <v>1</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H42" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="30" customHeight="1">
       <c r="A43" s="53" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B43" s="55" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="E43" s="4">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="E43" s="8">
+        <v>13</v>
       </c>
       <c r="F43" s="31">
         <v>1</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H43" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="30" hidden="1" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="30" customHeight="1">
       <c r="A44" s="53" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E44" s="4">
         <v>8</v>
@@ -4487,26 +4571,52 @@
         <v>1</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H44" s="44" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="I44" s="31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="30" customHeight="1">
+      <c r="A45" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="4">
+        <v>8</v>
+      </c>
+      <c r="F45" s="31">
+        <v>1</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="I45" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J44" xr:uid="{2F959334-FF27-4A0F-9E6B-19A8615EAC13}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Em andamento"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:J45" xr:uid="{2F959334-FF27-4A0F-9E6B-19A8615EAC13}"/>
   <mergeCells count="7">
     <mergeCell ref="L23:M23"/>
     <mergeCell ref="L26:M26"/>
@@ -4517,7 +4627,7 @@
     <mergeCell ref="L25:M25"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C3:C44">
+  <conditionalFormatting sqref="C3:C45">
     <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="Desejável">
       <formula>NOT(ISERROR(SEARCH("Desejável",C3)))</formula>
     </cfRule>
@@ -4528,7 +4638,7 @@
       <formula>NOT(ISERROR(SEARCH("Essencial",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D44">
+  <conditionalFormatting sqref="D3:D45">
     <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="PP">
       <formula>NOT(ISERROR(SEARCH("PP",D3)))</formula>
     </cfRule>
@@ -4545,7 +4655,7 @@
       <formula>NOT(ISERROR(SEARCH("P",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H44">
+  <conditionalFormatting sqref="H3:H45">
     <cfRule type="containsText" dxfId="35" priority="9" operator="containsText" text="Pendente">
       <formula>NOT(ISERROR(SEARCH("Pendente",H3)))</formula>
     </cfRule>
@@ -4557,13 +4667,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H44" xr:uid="{57770960-B32A-4E77-8824-5E34729DA2D1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H35:H45 H3:H34" xr:uid="{57770960-B32A-4E77-8824-5E34729DA2D1}">
       <formula1>"Feito,Em andamento,Pendente"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D44" xr:uid="{46B54BAF-FF80-4DEE-882A-3CFF59A27D0D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D35:D45 D3:D34" xr:uid="{46B54BAF-FF80-4DEE-882A-3CFF59A27D0D}">
       <formula1>"PP,P,M,G,GG"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C44" xr:uid="{12338359-4C07-4F0B-9395-A91D677B2843}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C35:C45 C3:C34" xr:uid="{12338359-4C07-4F0B-9395-A91D677B2843}">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4596,7 +4706,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="27" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -4610,25 +4720,25 @@
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
@@ -4637,22 +4747,22 @@
         <v>9</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="K2" s="58"/>
     </row>
     <row r="3" spans="1:11" ht="35.1" customHeight="1">
       <c r="A3" s="24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8">
         <v>5</v>
@@ -4661,31 +4771,31 @@
         <v>3</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="K3" s="58"/>
     </row>
     <row r="4" spans="1:11" ht="35.1" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E4" s="9">
         <v>21</v>
@@ -4694,31 +4804,31 @@
         <v>1</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="K4" s="58"/>
     </row>
     <row r="5" spans="1:11" ht="35.1" customHeight="1">
       <c r="A5" s="24" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E5" s="9">
         <v>8</v>
@@ -4727,30 +4837,30 @@
         <v>2</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J5" s="57" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="35.1" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8">
         <v>13</v>
@@ -4759,31 +4869,31 @@
         <v>2</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="K6" s="58"/>
     </row>
     <row r="7" spans="1:11" ht="35.1" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E7" s="13">
         <v>21</v>
@@ -4792,31 +4902,31 @@
         <v>1</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="K7" s="58"/>
     </row>
     <row r="8" spans="1:11" ht="35.1" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>8</v>
@@ -4825,31 +4935,31 @@
         <v>3</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" ht="35.1" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="E9" s="5">
         <v>21</v>
@@ -4858,30 +4968,30 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="35.1" customHeight="1">
       <c r="A10" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="42" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>80</v>
       </c>
       <c r="E10" s="4">
         <v>21</v>
@@ -4890,30 +5000,30 @@
         <v>2</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="35.1" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E11" s="5">
         <v>8</v>
@@ -4922,30 +5032,30 @@
         <v>2</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="35.1" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E12" s="17">
         <v>8</v>
@@ -4954,16 +5064,16 @@
         <v>3</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H12" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -5061,7 +5171,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -5075,25 +5185,25 @@
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
@@ -5102,21 +5212,21 @@
         <v>9</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="35.1" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E3" s="17">
         <v>8</v>
@@ -5125,33 +5235,33 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="35.1" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E4" s="17">
         <v>8</v>
@@ -5160,33 +5270,33 @@
         <v>2</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="35.1" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E5" s="8">
         <v>13</v>
@@ -5195,33 +5305,33 @@
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="J5" s="12" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="K5" s="49" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="35.1" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8">
         <v>13</v>
@@ -5230,33 +5340,33 @@
         <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="J6" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="K6" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="35.1" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E7" s="8">
         <v>13</v>
@@ -5265,33 +5375,33 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="K7" s="45" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="35.1" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E8" s="8">
         <v>13</v>
@@ -5300,33 +5410,33 @@
         <v>2</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="35.1" customHeight="1">
       <c r="A9" s="26" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E9" s="8">
         <v>13</v>
@@ -5335,30 +5445,30 @@
         <v>2</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>34</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="35.1" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E10" s="17">
         <v>8</v>
@@ -5367,30 +5477,30 @@
         <v>1</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="35.1" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4">
         <v>8</v>
@@ -5399,30 +5509,30 @@
         <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="35.1" customHeight="1">
       <c r="A12" s="26" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E12" s="8">
         <v>13</v>
@@ -5431,30 +5541,30 @@
         <v>1</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H12" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="35.1" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E13" s="17">
         <v>8</v>
@@ -5463,30 +5573,30 @@
         <v>3</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H13" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="35.1" customHeight="1">
       <c r="A14" s="26" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E14" s="8">
         <v>13</v>
@@ -5495,30 +5605,30 @@
         <v>1</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H14" s="44" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="35.1" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E15" s="8">
         <v>13</v>
@@ -5527,30 +5637,30 @@
         <v>2</v>
       </c>
       <c r="G15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="J15" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="35.1" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E16" s="17">
         <v>8</v>
@@ -5559,30 +5669,30 @@
         <v>3</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H16" s="44" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="35.1" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E17" s="8">
         <v>13</v>
@@ -5591,16 +5701,16 @@
         <v>1</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -5682,7 +5792,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="24.95" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -5696,25 +5806,25 @@
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
@@ -5723,21 +5833,21 @@
         <v>9</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4">
         <v>8</v>
@@ -5746,30 +5856,30 @@
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I3" s="31" t="s">
         <v>34</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4">
         <v>8</v>
@@ -5778,30 +5888,30 @@
         <v>1</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E5" s="8">
         <v>13</v>
@@ -5810,30 +5920,30 @@
         <v>1</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4">
         <v>8</v>
@@ -5842,30 +5952,30 @@
         <v>1</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I6" s="31" t="s">
         <v>34</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1">
       <c r="A7" s="53" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E7" s="4">
         <v>8</v>
@@ -5874,30 +5984,30 @@
         <v>1</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1">
       <c r="A8" s="53" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>8</v>
@@ -5906,30 +6016,30 @@
         <v>1</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1">
       <c r="A9" s="53" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4">
         <v>8</v>
@@ -5938,30 +6048,30 @@
         <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1">
       <c r="A10" s="53" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E10" s="8">
         <v>13</v>
@@ -5970,30 +6080,30 @@
         <v>1</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H10" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1">
       <c r="A11" s="53" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E11" s="8">
         <v>13</v>
@@ -6002,30 +6112,30 @@
         <v>1</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>34</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1">
       <c r="A12" s="53" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E12" s="4">
         <v>8</v>
@@ -6034,30 +6144,30 @@
         <v>1</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H12" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1">
       <c r="A13" s="53" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E13" s="8">
         <v>13</v>
@@ -6066,30 +6176,30 @@
         <v>1</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H13" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1">
       <c r="A14" s="53" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B14" s="55" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E14" s="4">
         <v>8</v>
@@ -6098,30 +6208,30 @@
         <v>1</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H14" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1">
       <c r="A15" s="53" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="E15" s="8">
         <v>5</v>
@@ -6130,30 +6240,30 @@
         <v>1</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H15" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="53" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E16" s="8">
         <v>13</v>
@@ -6162,30 +6272,30 @@
         <v>1</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H16" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1">
       <c r="A17" s="53" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="E17" s="8">
         <v>13</v>
@@ -6194,30 +6304,30 @@
         <v>1</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I17" s="31" t="s">
         <v>34</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="53" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="B18" s="55" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E18" s="4">
         <v>8</v>
@@ -6226,30 +6336,30 @@
         <v>1</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H18" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1">
       <c r="A19" s="53" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4">
         <v>8</v>
@@ -6258,16 +6368,16 @@
         <v>1</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>